<commit_message>
Aggiornata checklist con dati aggiornati
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ONIT0000000/OnitGroup/SIRVa/V.4.42.0.0/accreditamento-checklist_V4.2.xlsx
+++ b/GATEWAY/S1#111ONIT0000000/OnitGroup/SIRVa/V.4.42.0.0/accreditamento-checklist_V4.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afusaroli\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\FSE 2.0\it-fse-accreditamento-main\GATEWAY\S1#111ONIT0000000\OnitGroup\SIRVa\V.4.42.0.0\4-Certificato Vaccinale\Test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC275E8-E45A-4D32-8438-82697B211C59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6444E06-B2B2-4BCE-96A9-A65189C4039A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -1901,78 +1901,9 @@
     <t>subject_application_id:SIRVa</t>
   </si>
   <si>
-    <t>2023-02-08T10:29:06Z</t>
-  </si>
-  <si>
-    <t>387edac49bc90186</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.301.4.4.18f93001cf43131d4ddd4aa7d9033052325fac194b272c5ce7731e6ef3cf036f.f2bc4cea83^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-08T10:37:50Z</t>
-  </si>
-  <si>
-    <t>b0ff5cde9ed8d47d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.301.4.4.167d91771de940cb0bdf4f18ab87e314547613a170b46c6735d026801c544687.968e5067df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-08T10:55:30Z</t>
-  </si>
-  <si>
-    <t>1885e476c1b92014</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.301.4.4.b7dbff4495e09e3a58b4fe30bfb35e193daf31b09fa087f1a20ad37f001ecb5b.5f5fbab28c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-08T11:33:44Z</t>
-  </si>
-  <si>
-    <t>46535bc1f4360b76</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.301.4.4.486de6ec417a5e210c978267b0d1ef467bebc88245de0a693a615bd80b48537a.9f86a71cef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-02-08T15:08:20Z</t>
-  </si>
-  <si>
-    <t>c31d9e9d2bf4c615</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.301.4.4.1dfb0b67e4e771502b6fbc5c19319c2d9052a489bfc5c9a64e238b1124bc1cb0.a772b4ba51^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-08T15:17:01Z</t>
-  </si>
-  <si>
-    <t>9a7269de3329ac4b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.301.4.4.7da145ed84d814f754d76a359658b40e66bd5c82887b040ce3e3a9f76dc9063f.e800317ebd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-08T15:24:17Z</t>
-  </si>
-  <si>
-    <t>747fd01e7f4bae12</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.301.4.4.3ed1bf8f9fb51f1798244223dabd1cde5cbea4e54d51e045966ce72511133f06.61f88edfe7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-08T15:31:49Z</t>
-  </si>
-  <si>
-    <t>35e5fda7d8cd3d37</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.301.4.4.622fa203554d3544da2eb20abaa415e69d7234adbbd7237c31944f2dd8af5239.9aea0a543d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-02-08T11:42:55Z</t>
   </si>
   <si>
@@ -2160,6 +2091,75 @@
   </si>
   <si>
     <t>subject_application_version: V.4.42.0.0</t>
+  </si>
+  <si>
+    <t>7afd7f499a530345</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.301.4.4.18f93001cf43131d4ddd4aa7d9033052325fac194b272c5ce7731e6ef3cf036f.ccbac8b49e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-08T12:16:47Z</t>
+  </si>
+  <si>
+    <t>2023-03-08T12:22:14Z</t>
+  </si>
+  <si>
+    <t>df66e0f21bb0bbcf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.301.4.4.167d91771de940cb0bdf4f18ab87e314547613a170b46c6735d026801c544687.7c70bafed9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>434f3db5e58f65d7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.301.4.4.b7dbff4495e09e3a58b4fe30bfb35e193daf31b09fa087f1a20ad37f001ecb5b.e2189cc949^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-08T12:27:25Z</t>
+  </si>
+  <si>
+    <t>ac00a7442a55b09d</t>
+  </si>
+  <si>
+    <t>2023-03-08T12:30:01Z</t>
+  </si>
+  <si>
+    <t>c9191232e58c8aa3</t>
+  </si>
+  <si>
+    <t>2023-03-08T14:14:27Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.301.4.4.1dfb0b67e4e771502b6fbc5c19319c2d9052a489bfc5c9a64e238b1124bc1cb0.b5cb235f22^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f71f01413dbffd9d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.301.4.4.7da145ed84d814f754d76a359658b40e66bd5c82887b040ce3e3a9f76dc9063f.bb91af4214^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-08T14:17:44Z</t>
+  </si>
+  <si>
+    <t>09c66b9575030a8c</t>
+  </si>
+  <si>
+    <t>2023-03-08T14:20:19Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.301.4.4.3ed1bf8f9fb51f1798244223dabd1cde5cbea4e54d51e045966ce72511133f06.b059f6754b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-08T14:22:33Z</t>
+  </si>
+  <si>
+    <t>c9b700f82459bf75</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.301.4.4.622fa203554d3544da2eb20abaa415e69d7234adbbd7237c31944f2dd8af5239.1585cab492^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4315,10 +4315,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B118" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:D5"/>
+      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4369,7 +4369,7 @@
       </c>
       <c r="B2" s="57"/>
       <c r="C2" s="58" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
       <c r="D2" s="57"/>
       <c r="F2" s="27"/>
@@ -4441,7 +4441,7 @@
       <c r="A5" s="63"/>
       <c r="B5" s="64"/>
       <c r="C5" s="65" t="s">
-        <v>427</v>
+        <v>404</v>
       </c>
       <c r="D5" s="57"/>
       <c r="F5" s="27"/>
@@ -5038,16 +5038,16 @@
         <v>57</v>
       </c>
       <c r="F23" s="48">
-        <v>44965</v>
+        <v>44993</v>
       </c>
       <c r="G23" s="49" t="s">
-        <v>341</v>
+        <v>407</v>
       </c>
       <c r="H23" s="49" t="s">
-        <v>342</v>
+        <v>405</v>
       </c>
       <c r="I23" s="49" t="s">
-        <v>343</v>
+        <v>406</v>
       </c>
       <c r="J23" s="41" t="s">
         <v>84</v>
@@ -5082,16 +5082,16 @@
         <v>59</v>
       </c>
       <c r="F24" s="48">
-        <v>44965</v>
+        <v>44993</v>
       </c>
       <c r="G24" s="49" t="s">
-        <v>344</v>
+        <v>408</v>
       </c>
       <c r="H24" s="50" t="s">
-        <v>345</v>
+        <v>409</v>
       </c>
       <c r="I24" s="49" t="s">
-        <v>346</v>
+        <v>410</v>
       </c>
       <c r="J24" s="41" t="s">
         <v>84</v>
@@ -5126,16 +5126,16 @@
         <v>61</v>
       </c>
       <c r="F25" s="48">
-        <v>44965</v>
+        <v>44993</v>
       </c>
       <c r="G25" s="49" t="s">
-        <v>347</v>
+        <v>413</v>
       </c>
       <c r="H25" s="50" t="s">
-        <v>348</v>
+        <v>411</v>
       </c>
       <c r="I25" s="49" t="s">
-        <v>349</v>
+        <v>412</v>
       </c>
       <c r="J25" s="41" t="s">
         <v>84</v>
@@ -5170,16 +5170,16 @@
         <v>63</v>
       </c>
       <c r="F26" s="48">
-        <v>44965</v>
+        <v>44993</v>
       </c>
       <c r="G26" s="49" t="s">
-        <v>350</v>
+        <v>415</v>
       </c>
       <c r="H26" s="49" t="s">
-        <v>351</v>
+        <v>414</v>
       </c>
       <c r="I26" s="49" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="J26" s="41" t="s">
         <v>84</v>
@@ -5214,16 +5214,16 @@
         <v>66</v>
       </c>
       <c r="F27" s="48">
-        <v>44965</v>
+        <v>44993</v>
       </c>
       <c r="G27" s="49" t="s">
-        <v>353</v>
+        <v>417</v>
       </c>
       <c r="H27" s="49" t="s">
-        <v>354</v>
+        <v>416</v>
       </c>
       <c r="I27" s="49" t="s">
-        <v>355</v>
+        <v>418</v>
       </c>
       <c r="J27" s="41" t="s">
         <v>84</v>
@@ -5258,16 +5258,16 @@
         <v>68</v>
       </c>
       <c r="F28" s="48">
-        <v>44965</v>
+        <v>44993</v>
       </c>
       <c r="G28" s="49" t="s">
-        <v>356</v>
+        <v>421</v>
       </c>
       <c r="H28" s="49" t="s">
-        <v>357</v>
+        <v>419</v>
       </c>
       <c r="I28" s="49" t="s">
-        <v>358</v>
+        <v>420</v>
       </c>
       <c r="J28" s="41" t="s">
         <v>84</v>
@@ -5302,16 +5302,16 @@
         <v>70</v>
       </c>
       <c r="F29" s="48">
-        <v>44965</v>
+        <v>44993</v>
       </c>
       <c r="G29" s="49" t="s">
-        <v>359</v>
+        <v>423</v>
       </c>
       <c r="H29" s="49" t="s">
-        <v>360</v>
+        <v>422</v>
       </c>
       <c r="I29" s="49" t="s">
-        <v>361</v>
+        <v>424</v>
       </c>
       <c r="J29" s="41" t="s">
         <v>84</v>
@@ -5346,16 +5346,16 @@
         <v>72</v>
       </c>
       <c r="F30" s="48">
-        <v>44965</v>
+        <v>44993</v>
       </c>
       <c r="G30" s="49" t="s">
-        <v>362</v>
+        <v>425</v>
       </c>
       <c r="H30" s="49" t="s">
-        <v>363</v>
+        <v>426</v>
       </c>
       <c r="I30" s="49" t="s">
-        <v>364</v>
+        <v>427</v>
       </c>
       <c r="J30" s="41" t="s">
         <v>84</v>
@@ -5631,13 +5631,13 @@
         <v>44965</v>
       </c>
       <c r="G38" s="49" t="s">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="H38" s="49" t="s">
-        <v>366</v>
+        <v>343</v>
       </c>
       <c r="I38" s="49" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="J38" s="41" t="s">
         <v>84</v>
@@ -5654,7 +5654,7 @@
         <v>84</v>
       </c>
       <c r="P38" s="51" t="s">
-        <v>368</v>
+        <v>345</v>
       </c>
       <c r="Q38" s="41"/>
       <c r="R38" s="44"/>
@@ -5683,13 +5683,13 @@
         <v>44965</v>
       </c>
       <c r="G39" s="49" t="s">
-        <v>369</v>
+        <v>346</v>
       </c>
       <c r="H39" s="49" t="s">
-        <v>370</v>
+        <v>347</v>
       </c>
       <c r="I39" s="49" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="J39" s="41" t="s">
         <v>84</v>
@@ -5706,7 +5706,7 @@
         <v>84</v>
       </c>
       <c r="P39" s="51" t="s">
-        <v>371</v>
+        <v>348</v>
       </c>
       <c r="Q39" s="41"/>
       <c r="R39" s="44"/>
@@ -5871,13 +5871,13 @@
         <v>44965</v>
       </c>
       <c r="G44" s="49" t="s">
-        <v>372</v>
+        <v>349</v>
       </c>
       <c r="H44" s="49" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="I44" s="49" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="J44" s="41" t="s">
         <v>84</v>
@@ -5894,7 +5894,7 @@
         <v>84</v>
       </c>
       <c r="P44" s="41" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
       <c r="Q44" s="41"/>
       <c r="R44" s="44"/>
@@ -5923,13 +5923,13 @@
         <v>44965</v>
       </c>
       <c r="G45" s="49" t="s">
-        <v>375</v>
+        <v>352</v>
       </c>
       <c r="H45" s="49" t="s">
-        <v>376</v>
+        <v>353</v>
       </c>
       <c r="I45" s="49" t="s">
-        <v>367</v>
+        <v>344</v>
       </c>
       <c r="J45" s="41" t="s">
         <v>84</v>
@@ -5946,7 +5946,7 @@
         <v>84</v>
       </c>
       <c r="P45" s="51" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
       <c r="Q45" s="41"/>
       <c r="R45" s="44"/>
@@ -6126,7 +6126,7 @@
       <c r="N50" s="41"/>
       <c r="O50" s="41"/>
       <c r="P50" s="41" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
       <c r="Q50" s="41"/>
       <c r="R50" s="44" t="s">
@@ -6166,7 +6166,7 @@
       <c r="N51" s="41"/>
       <c r="O51" s="41"/>
       <c r="P51" s="51" t="s">
-        <v>377</v>
+        <v>354</v>
       </c>
       <c r="Q51" s="41"/>
       <c r="R51" s="44" t="s">
@@ -7665,7 +7665,7 @@
         <v>321</v>
       </c>
       <c r="K95" s="41" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
       <c r="L95" s="41"/>
       <c r="M95" s="41"/>
@@ -7703,7 +7703,7 @@
         <v>321</v>
       </c>
       <c r="K96" s="41" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="L96" s="41"/>
       <c r="M96" s="41"/>
@@ -7741,7 +7741,7 @@
         <v>321</v>
       </c>
       <c r="K97" s="41" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="L97" s="41"/>
       <c r="M97" s="41"/>
@@ -7775,13 +7775,13 @@
         <v>44965</v>
       </c>
       <c r="G98" s="49" t="s">
-        <v>381</v>
+        <v>358</v>
       </c>
       <c r="H98" s="49" t="s">
-        <v>382</v>
+        <v>359</v>
       </c>
       <c r="I98" s="49" t="s">
-        <v>383</v>
+        <v>360</v>
       </c>
       <c r="J98" s="41" t="s">
         <v>84</v>
@@ -7798,7 +7798,7 @@
         <v>84</v>
       </c>
       <c r="P98" s="41" t="s">
-        <v>384</v>
+        <v>361</v>
       </c>
       <c r="Q98" s="41"/>
       <c r="R98" s="44"/>
@@ -7831,7 +7831,7 @@
         <v>321</v>
       </c>
       <c r="K99" s="41" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="L99" s="41"/>
       <c r="M99" s="41"/>
@@ -7869,7 +7869,7 @@
         <v>321</v>
       </c>
       <c r="K100" s="41" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="L100" s="41"/>
       <c r="M100" s="41"/>
@@ -7907,7 +7907,7 @@
         <v>321</v>
       </c>
       <c r="K101" s="41" t="s">
-        <v>387</v>
+        <v>364</v>
       </c>
       <c r="L101" s="41"/>
       <c r="M101" s="41"/>
@@ -7945,7 +7945,7 @@
         <v>321</v>
       </c>
       <c r="K102" s="41" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="L102" s="41"/>
       <c r="M102" s="41"/>
@@ -7979,13 +7979,13 @@
         <v>44965</v>
       </c>
       <c r="G103" s="49" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="H103" s="49" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="I103" s="49" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
       <c r="J103" s="41" t="s">
         <v>84</v>
@@ -8002,7 +8002,7 @@
         <v>84</v>
       </c>
       <c r="P103" s="52" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
       <c r="Q103" s="41"/>
       <c r="R103" s="44"/>
@@ -8035,7 +8035,7 @@
         <v>321</v>
       </c>
       <c r="K104" s="41" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="L104" s="41"/>
       <c r="M104" s="41"/>
@@ -8069,13 +8069,13 @@
         <v>44965</v>
       </c>
       <c r="G105" s="49" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="H105" s="49" t="s">
-        <v>396</v>
+        <v>373</v>
       </c>
       <c r="I105" s="49" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="J105" s="41" t="s">
         <v>84</v>
@@ -8092,7 +8092,7 @@
         <v>84</v>
       </c>
       <c r="P105" s="52" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
       <c r="Q105" s="41"/>
       <c r="R105" s="44"/>
@@ -8125,7 +8125,7 @@
         <v>321</v>
       </c>
       <c r="K106" s="41" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="L106" s="41"/>
       <c r="M106" s="41"/>
@@ -8159,16 +8159,16 @@
         <v>44965</v>
       </c>
       <c r="G107" s="49" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
       <c r="H107" s="49" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
       <c r="I107" s="49" t="s">
-        <v>402</v>
+        <v>379</v>
       </c>
       <c r="J107" s="41" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="K107" s="41"/>
       <c r="L107" s="41" t="s">
@@ -8182,7 +8182,7 @@
         <v>84</v>
       </c>
       <c r="P107" s="41" t="s">
-        <v>404</v>
+        <v>381</v>
       </c>
       <c r="Q107" s="41"/>
       <c r="R107" s="44"/>
@@ -8215,7 +8215,7 @@
         <v>321</v>
       </c>
       <c r="K108" s="41" t="s">
-        <v>405</v>
+        <v>382</v>
       </c>
       <c r="L108" s="41"/>
       <c r="M108" s="41"/>
@@ -8253,7 +8253,7 @@
         <v>321</v>
       </c>
       <c r="K109" s="41" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="L109" s="41"/>
       <c r="M109" s="41"/>
@@ -8291,7 +8291,7 @@
         <v>321</v>
       </c>
       <c r="K110" s="41" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="L110" s="41"/>
       <c r="M110" s="41"/>
@@ -8325,13 +8325,13 @@
         <v>44965</v>
       </c>
       <c r="G111" s="53" t="s">
-        <v>406</v>
+        <v>383</v>
       </c>
       <c r="H111" s="49" t="s">
-        <v>407</v>
+        <v>384</v>
       </c>
       <c r="I111" s="49" t="s">
-        <v>408</v>
+        <v>385</v>
       </c>
       <c r="J111" s="41" t="s">
         <v>84</v>
@@ -8348,7 +8348,7 @@
         <v>84</v>
       </c>
       <c r="P111" s="41" t="s">
-        <v>384</v>
+        <v>361</v>
       </c>
       <c r="Q111" s="41"/>
       <c r="R111" s="44"/>
@@ -8381,7 +8381,7 @@
         <v>321</v>
       </c>
       <c r="K112" s="41" t="s">
-        <v>385</v>
+        <v>362</v>
       </c>
       <c r="L112" s="41"/>
       <c r="M112" s="41"/>
@@ -8419,7 +8419,7 @@
         <v>321</v>
       </c>
       <c r="K113" s="41" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="L113" s="41"/>
       <c r="M113" s="41"/>
@@ -8457,7 +8457,7 @@
         <v>321</v>
       </c>
       <c r="K114" s="41" t="s">
-        <v>425</v>
+        <v>402</v>
       </c>
       <c r="L114" s="41"/>
       <c r="M114" s="41"/>
@@ -8491,13 +8491,13 @@
         <v>44965</v>
       </c>
       <c r="G115" s="49" t="s">
-        <v>409</v>
+        <v>386</v>
       </c>
       <c r="H115" s="49" t="s">
-        <v>410</v>
+        <v>387</v>
       </c>
       <c r="I115" s="49" t="s">
-        <v>411</v>
+        <v>388</v>
       </c>
       <c r="J115" s="41" t="s">
         <v>84</v>
@@ -8514,7 +8514,7 @@
         <v>84</v>
       </c>
       <c r="P115" s="41" t="s">
-        <v>412</v>
+        <v>389</v>
       </c>
       <c r="Q115" s="41"/>
       <c r="R115" s="44"/>
@@ -8547,7 +8547,7 @@
         <v>321</v>
       </c>
       <c r="K116" s="41" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="L116" s="41"/>
       <c r="M116" s="41"/>
@@ -8581,13 +8581,13 @@
         <v>44965</v>
       </c>
       <c r="G117" s="49" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
       <c r="H117" s="49" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
       <c r="I117" s="49" t="s">
-        <v>415</v>
+        <v>392</v>
       </c>
       <c r="J117" s="41" t="s">
         <v>84</v>
@@ -8604,7 +8604,7 @@
         <v>84</v>
       </c>
       <c r="P117" s="41" t="s">
-        <v>416</v>
+        <v>393</v>
       </c>
       <c r="Q117" s="41"/>
       <c r="R117" s="44"/>
@@ -8637,7 +8637,7 @@
         <v>321</v>
       </c>
       <c r="K118" s="41" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="L118" s="41"/>
       <c r="M118" s="41"/>
@@ -8671,13 +8671,13 @@
         <v>44965</v>
       </c>
       <c r="G119" s="49" t="s">
-        <v>417</v>
+        <v>394</v>
       </c>
       <c r="H119" s="49" t="s">
-        <v>418</v>
+        <v>395</v>
       </c>
       <c r="I119" s="49" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
       <c r="J119" s="41" t="s">
         <v>84</v>
@@ -8694,7 +8694,7 @@
         <v>84</v>
       </c>
       <c r="P119" s="41" t="s">
-        <v>420</v>
+        <v>397</v>
       </c>
       <c r="Q119" s="41"/>
       <c r="R119" s="44"/>
@@ -8727,7 +8727,7 @@
         <v>321</v>
       </c>
       <c r="K120" s="41" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="L120" s="41"/>
       <c r="M120" s="41"/>
@@ -8765,7 +8765,7 @@
         <v>321</v>
       </c>
       <c r="K121" s="41" t="s">
-        <v>421</v>
+        <v>398</v>
       </c>
       <c r="L121" s="41"/>
       <c r="M121" s="41"/>
@@ -8799,13 +8799,13 @@
         <v>44965</v>
       </c>
       <c r="G122" s="49" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
       <c r="H122" s="49" t="s">
-        <v>423</v>
+        <v>400</v>
       </c>
       <c r="I122" s="49" t="s">
-        <v>424</v>
+        <v>401</v>
       </c>
       <c r="J122" s="41" t="s">
         <v>84</v>
@@ -8822,7 +8822,7 @@
         <v>84</v>
       </c>
       <c r="P122" s="52" t="s">
-        <v>420</v>
+        <v>397</v>
       </c>
       <c r="Q122" s="41"/>
       <c r="R122" s="44"/>
@@ -26261,17 +26261,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -26280,7 +26269,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -26511,24 +26500,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -26536,7 +26519,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26555,6 +26538,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>